<commit_message>
workbook, worksheets 방식 사용
</commit_message>
<xml_diff>
--- a/WPF_Tranning/Resources/output.xlsx
+++ b/WPF_Tranning/Resources/output.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m6ydz642\source\repos\WPF_Tranning\WPF_Tranning\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA7A093-2AFB-472C-8033-DFB61B3C40CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-19200" yWindow="0" windowWidth="14400" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">Sheet!$A$1:$C$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$C$32</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>체크박스</t>
   </si>
@@ -110,19 +121,30 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="m&quot;/&quot;d;@"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color auto="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -161,18 +183,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -438,377 +471,382 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane topLeftCell="A2" ySplit="1" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1:A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="14.29" customWidth="1" style="1"/>
-    <col min="2" max="2" width="9.71" customWidth="1" style="2"/>
-    <col min="3" max="3" width="21.71" customWidth="1" style="1"/>
+    <col min="1" max="1" width="14.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.75" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c t="s" r="B1" s="1">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c t="b" r="A2" s="1">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c t="s" r="C2" s="1">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c t="b" r="A3" s="1">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c t="s" r="C3" s="1">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c t="b" r="A4" s="1">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c t="s" r="C4" s="1">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c t="b" r="A5" s="1">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c t="s" r="C5" s="1">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6">
-      <c t="b" r="A6" s="1">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c t="s" r="C6" s="1">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c t="b" r="A7" s="1">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c t="s" r="C7" s="1">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8">
-      <c t="b" r="A8" s="1">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c t="s" r="C8" s="1">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9">
-      <c t="b" r="A9" s="1">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B9" s="2">
         <v>13</v>
       </c>
-      <c t="s" r="C9" s="1">
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10">
-      <c t="b" r="A10" s="1">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B10" s="2">
         <v>14</v>
       </c>
-      <c t="s" r="C10" s="1">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11">
-      <c t="b" r="A11" s="1">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B11" s="2">
         <v>1055</v>
       </c>
-      <c t="s" r="C11" s="1">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c t="b" r="A12" s="1">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B12" s="2">
         <v>1056</v>
       </c>
-      <c t="s" r="C12" s="1">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13">
-      <c t="b" r="A13" s="1">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B13" s="2">
         <v>1057</v>
       </c>
-      <c t="s" r="C13" s="1">
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14">
-      <c t="b" r="A14" s="1">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B14" s="2">
         <v>1058</v>
       </c>
-      <c t="s" r="C14" s="1">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15">
-      <c t="b" r="A15" s="1">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B15" s="2">
         <v>1059</v>
       </c>
-      <c t="s" r="C15" s="1">
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16">
-      <c t="b" r="A16" s="1">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B16" s="2">
         <v>1063</v>
       </c>
-      <c t="s" r="C16" s="1">
+      <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17">
-      <c t="b" r="A17" s="1">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B17" s="2">
         <v>1065</v>
       </c>
-      <c t="s" r="C17" s="1">
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18">
-      <c t="b" r="A18" s="1">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B18" s="2">
         <v>1066</v>
       </c>
-      <c t="s" r="C18" s="1">
+      <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19">
-      <c t="b" r="A19" s="1">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B19" s="2">
         <v>1067</v>
       </c>
-      <c t="s" r="C19" s="1">
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20">
-      <c t="b" r="A20" s="1">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B20" s="2">
         <v>1068</v>
       </c>
-      <c t="s" r="C20" s="1">
+      <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21">
-      <c t="b" r="A21" s="1">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B21" s="2">
         <v>1069</v>
       </c>
-      <c t="s" r="C21" s="1">
+      <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22">
-      <c t="b" r="A22" s="1">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B22" s="2">
         <v>1070</v>
       </c>
-      <c t="s" r="C22" s="1">
+      <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23">
-      <c t="b" r="A23" s="1">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B23" s="2">
         <v>1072</v>
       </c>
-      <c t="s" r="C23" s="1">
+      <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24">
-      <c t="b" r="A24" s="1">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B24" s="2">
         <v>9</v>
       </c>
-      <c t="s" r="C24" s="1">
+      <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25">
-      <c t="b" r="A25" s="1">
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B25" s="2">
         <v>10</v>
       </c>
-      <c t="s" r="C25" s="1">
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26">
-      <c t="b" r="A26" s="1">
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B26" s="2">
         <v>12</v>
       </c>
-      <c t="s" r="C26" s="1">
+      <c r="C26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27">
-      <c t="b" r="A27" s="1">
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B27" s="2">
         <v>1054</v>
       </c>
-      <c t="s" r="C27" s="1">
+      <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28">
-      <c t="b" r="A28" s="1">
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B28" s="2">
         <v>1060</v>
       </c>
-      <c t="s" r="C28" s="1">
+      <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29">
-      <c t="b" r="A29" s="1">
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B29" s="2">
         <v>1061</v>
       </c>
-      <c t="s" r="C29" s="1">
+      <c r="C29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30">
-      <c t="b" r="A30" s="1">
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B30" s="2">
         <v>1062</v>
       </c>
-      <c t="s" r="C30" s="1">
+      <c r="C30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31">
-      <c t="b" r="A31" s="1">
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B31" s="2">
         <v>1071</v>
       </c>
-      <c t="s" r="C31" s="1">
+      <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32">
-      <c t="b" r="A32" s="1">
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="B32" s="2">
         <v>1064</v>
       </c>
-      <c t="s" r="C32" s="1">
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C32"/>
-  <pageSetup fitToWidth="0" fitToHeight="0"/>
+  <autoFilter ref="A1:C32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:C32" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>